<commit_message>
Game dice game following evaluations done: only_semantic_smells, only_syntactic_smells, random_01, random_02. all_smells and no_smells evaluations hotfix.
</commit_message>
<xml_diff>
--- a/evaluations/GPT/2025-04-05_094619/dice_game/all_smells_01/evaluation.xlsx
+++ b/evaluations/GPT/2025-04-05_094619/dice_game/all_smells_01/evaluation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -85,7 +85,7 @@
     <t>negative</t>
   </si>
   <si>
-    <t>2.3.1, 2.5.3</t>
+    <t>2.3.1</t>
   </si>
   <si>
     <t>numerical_discrepancies</t>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>1.3, 1.4</t>
-  </si>
-  <si>
-    <t>2.3.1</t>
   </si>
   <si>
     <t>weak_verbs</t>
@@ -834,7 +831,7 @@
         <v>0.0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -848,13 +845,13 @@
         <v>13</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F21" s="1">
         <v>0.0</v>
@@ -880,7 +877,7 @@
         <v>0.0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="1">
         <v>1.0</v>
@@ -920,7 +917,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1">
         <v>1.0</v>
@@ -988,7 +985,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>

</xml_diff>